<commit_message>
Subi arquivos usados para gerar o relatório de inadimplentes
</commit_message>
<xml_diff>
--- a/dados/cef/inadimplentes/grauçá.xlsx
+++ b/dados/cef/inadimplentes/grauçá.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t/>
   </si>
@@ -22,10 +22,10 @@
     <t>Folha No 1</t>
   </si>
   <si>
-    <t>Relatório de Inadimplência - Data de Referência: 05/03/2025</t>
-  </si>
-  <si>
-    <t>Impresso em: 05/03/2025 11:25:52</t>
+    <t>Relatório de Inadimplência - Data de Referência: 03/04/2025</t>
+  </si>
+  <si>
+    <t>Impresso em: 03/04/2025 16:46:09</t>
   </si>
   <si>
     <t>Título</t>
@@ -79,25 +79,25 @@
     <t>Empreendimento: GRA010001 - Up Select Vila Sônia</t>
   </si>
   <si>
-    <t>Cliente: VANDERSON NOGUEIRA MELO</t>
-  </si>
-  <si>
-    <t>Contrato: 0131-0</t>
-  </si>
-  <si>
-    <t>Telefones: +55  (0xx11)96052-7147</t>
-  </si>
-  <si>
-    <t>Unidade: Up Select Vila Sônia, Décimo quarto pavimento, Apartamento 1402</t>
+    <t>Cliente: ANA CAROLINA PERRONE LEITE</t>
+  </si>
+  <si>
+    <t>Contrato: 0017-0</t>
+  </si>
+  <si>
+    <t>Telefones: +55  (0xx11)98878-8355</t>
+  </si>
+  <si>
+    <t>Unidade: Up Select Vila Sônia, Sétimo pavimento, Apartamento 707</t>
   </si>
   <si>
     <t>Imobiliaria/Corretor:</t>
   </si>
   <si>
-    <t>25/01/2025</t>
-  </si>
-  <si>
-    <t>39</t>
+    <t>25/03/2025</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
   <si>
     <t>R</t>
@@ -106,73 +106,88 @@
     <t>NP</t>
   </si>
   <si>
-    <t>002/004</t>
-  </si>
-  <si>
-    <t>SIN</t>
-  </si>
-  <si>
-    <t>429,21</t>
+    <t>005/032</t>
+  </si>
+  <si>
+    <t>MEN</t>
+  </si>
+  <si>
+    <t>286,58</t>
   </si>
   <si>
     <t>0,00</t>
   </si>
   <si>
-    <t>3,33</t>
-  </si>
-  <si>
-    <t>5,62</t>
-  </si>
-  <si>
-    <t>8,65</t>
-  </si>
-  <si>
-    <t>446,81</t>
-  </si>
-  <si>
-    <t>003/004</t>
-  </si>
-  <si>
-    <t>25/02/2025</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>431,36</t>
-  </si>
-  <si>
-    <t>1,19</t>
-  </si>
-  <si>
-    <t>1,15</t>
-  </si>
-  <si>
-    <t>442,35</t>
-  </si>
-  <si>
-    <t>VANDERSON NOGUEIRA MELO: 2 Parcelas</t>
-  </si>
-  <si>
-    <t>889,16</t>
-  </si>
-  <si>
-    <t>860,57</t>
-  </si>
-  <si>
-    <t>4,52</t>
-  </si>
-  <si>
-    <t>6,77</t>
-  </si>
-  <si>
-    <t>17,30</t>
-  </si>
-  <si>
-    <t>Total: 1 Contrato em Atraso</t>
-  </si>
-  <si>
-    <t>Total Geral: 1 Contrato em Atraso</t>
+    <t>0,31</t>
+  </si>
+  <si>
+    <t>0,86</t>
+  </si>
+  <si>
+    <t>5,74</t>
+  </si>
+  <si>
+    <t>293,49</t>
+  </si>
+  <si>
+    <t>ANA CAROLINA PERRONE LEITE: 1 Parcela</t>
+  </si>
+  <si>
+    <t>Cliente: ELAINE SAMARA DA SILVA</t>
+  </si>
+  <si>
+    <t>Contrato: 0066-0</t>
+  </si>
+  <si>
+    <t>Telefones: +55  (0xx11)95867-6825</t>
+  </si>
+  <si>
+    <t>Unidade: Up Select Vila Sônia, Décimo terceiro pavimento, Apartamento 1306</t>
+  </si>
+  <si>
+    <t>20/03/2025</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>652,46</t>
+  </si>
+  <si>
+    <t>1,13</t>
+  </si>
+  <si>
+    <t>3,05</t>
+  </si>
+  <si>
+    <t>13,07</t>
+  </si>
+  <si>
+    <t>669,71</t>
+  </si>
+  <si>
+    <t>ELAINE SAMARA DA SILVA: 1 Parcela</t>
+  </si>
+  <si>
+    <t>Total: 2 Contratos em Atraso</t>
+  </si>
+  <si>
+    <t>939,04</t>
+  </si>
+  <si>
+    <t>1,44</t>
+  </si>
+  <si>
+    <t>3,91</t>
+  </si>
+  <si>
+    <t>18,81</t>
+  </si>
+  <si>
+    <t>963,20</t>
+  </si>
+  <si>
+    <t>Total Geral: 2 Contratos em Atraso</t>
   </si>
   <si>
     <t>Total Adesão Geral</t>
@@ -554,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="P4:L21"/>
+  <dimension ref="P4:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -574,7 +589,7 @@
       </c>
     </row>
     <row r="7" spans="2:14">
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -691,35 +706,20 @@
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="C14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>36</v>
@@ -728,109 +728,169 @@
         <v>33</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="I18" s="4" t="s">
+      <c r="K19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="I19" s="4" t="s">
+      <c r="M19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="I21" s="4" t="s">
+      <c r="N19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>46</v>
+      <c r="O19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="I22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="I23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="I24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1055,13 +1115,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343C58C6-E50F-42A6-9692-D9B3262EB098}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293F24E4-85A0-4A33-B518-865D6D937625}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF329C52-68F1-4A22-AA89-3F23FD71EAA6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71BCB428-44C2-468C-AFA4-B0E016DBA5D5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE8F5F5A-0424-48C0-8C01-6C001C94BDBD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C98B2C4-04BA-4AA3-886B-4FFD3C6E0077}"/>
 </file>
</xml_diff>